<commit_message>
Adding the 60Hz version.
</commit_message>
<xml_diff>
--- a/H2BR0-5/Rleased/BOM/H2BR0-5.xlsx
+++ b/H2BR0-5/Rleased/BOM/H2BR0-5.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HEXABITZ\Modules\Hardware\Modules Hardware Design\H2BR0x-Hardware\Rleased\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HEXABITZ\Modules\Hardware\Modules Hardware Design\H2BR0x-Hardware\H2BR0-5\Rleased\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D0FA1C-FFA1-43DF-9510-D2F53CDA2AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353DF9EB-87E5-4243-8DC7-A210F8E76886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="H2BR0" sheetId="1" r:id="rId1"/>
+    <sheet name="H2BR0-5" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="216">
   <si>
     <t>Description</t>
   </si>
@@ -310,12 +310,6 @@
     <t>CAB1</t>
   </si>
   <si>
-    <t>SENSOR CABLE - ELECTRODE PADS (3</t>
-  </si>
-  <si>
-    <t>https://octopart.com/cab-12970-sparkfun-76381356?r=sp</t>
-  </si>
-  <si>
     <t>TVS DIODE 3,3V 10,9V SOD323</t>
   </si>
   <si>
@@ -355,21 +349,12 @@
     <t>https://octopart.com/stm32g0b1ceu6-stmicroelectronics-116363364?r=sp</t>
   </si>
   <si>
-    <t>CAB-12970</t>
-  </si>
-  <si>
-    <t>SparkFun</t>
-  </si>
-  <si>
     <t>MPN</t>
   </si>
   <si>
     <t>MFN</t>
   </si>
   <si>
-    <t>TDK</t>
-  </si>
-  <si>
     <t>440054-3</t>
   </si>
   <si>
@@ -589,15 +574,6 @@
     <t>C8, C15, C16, C17, C18, C19, C20, C21</t>
   </si>
   <si>
-    <t>CAP 0402 0,1UF 16V TDK Multilayer Ceramic Capacitors MLCC-SMD/SMT</t>
-  </si>
-  <si>
-    <t>CGA2B1X7R1C104K050BC</t>
-  </si>
-  <si>
-    <t>https://octopart.com/cga2b1x7r1c104k050bc-tdk-26014376?r=sp</t>
-  </si>
-  <si>
     <t>CAP CER 0.1 UF 25V 10% X7R 0603</t>
   </si>
   <si>
@@ -677,6 +653,27 @@
   </si>
   <si>
     <t>https://octopart.com/cc0402krx5r6bb334-yageo-21548561</t>
+  </si>
+  <si>
+    <t>CC0402JRX7R7BB104</t>
+  </si>
+  <si>
+    <t>0.1 µF ±5% 16V Ceramic Capacitor X7R 0402 (1005 Metric)</t>
+  </si>
+  <si>
+    <t>https://octopart.com/cc0402jrx7r7bb104-yageo-21707045</t>
+  </si>
+  <si>
+    <t>https://www.alibaba.com/product-detail/Right-angle-Gold-plated-3-5mm_1600978965655.html?spm=a2700.picsearch.normal_offer.d_title.55b05f93R886wo</t>
+  </si>
+  <si>
+    <t>Right angle Gold plated 3.5mm Audio Plug to 3 Leads 3.5mm/4.0mm Female Electric Snap Connector ECG Cable</t>
+  </si>
+  <si>
+    <t>Alibaba</t>
+  </si>
+  <si>
+    <t>XR001650</t>
   </si>
 </sst>
 </file>
@@ -918,6 +915,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -938,9 +938,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -977,7 +974,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2368101</xdr:colOff>
+      <xdr:colOff>2377626</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>589597</xdr:rowOff>
     </xdr:to>
@@ -1319,8 +1316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1381,11 +1378,11 @@
       <c r="C4" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="23">
-        <v>1</v>
-      </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
+      <c r="D4" s="24">
+        <v>1</v>
+      </c>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
       <c r="G4" s="19"/>
     </row>
     <row r="5" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
@@ -1398,11 +1395,11 @@
       <c r="C5" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="25">
         <v>45670</v>
       </c>
-      <c r="E5" s="25"/>
-      <c r="F5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="27"/>
       <c r="G5" s="19"/>
     </row>
     <row r="6" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
@@ -1410,51 +1407,51 @@
         <v>8</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="29"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="30"/>
       <c r="G6" s="19"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="30" t="s">
+      <c r="A8" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="30" t="s">
-        <v>111</v>
-      </c>
-      <c r="D8" s="30" t="s">
-        <v>112</v>
-      </c>
-      <c r="E8" s="30" t="s">
+      <c r="C8" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="E8" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="30" t="s">
+      <c r="F8" s="23" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="21" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F9" s="6">
         <v>1</v>
@@ -1462,7 +1459,7 @@
     </row>
     <row r="10" spans="1:9" s="21" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>18</v>
@@ -1522,19 +1519,19 @@
     </row>
     <row r="13" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="F13" s="6">
         <v>1</v>
@@ -1562,7 +1559,7 @@
     </row>
     <row r="15" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>24</v>
@@ -1625,16 +1622,16 @@
         <v>43</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>64</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="F18" s="6">
         <v>1</v>
@@ -1645,16 +1642,16 @@
         <v>81</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>64</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="F19" s="6">
         <v>1</v>
@@ -1662,19 +1659,19 @@
     </row>
     <row r="20" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="F20" s="6">
         <v>2</v>
@@ -1685,16 +1682,16 @@
         <v>80</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>86</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F21" s="6">
         <v>2</v>
@@ -1705,16 +1702,16 @@
         <v>82</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>64</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="F22" s="6">
         <v>1</v>
@@ -1722,19 +1719,19 @@
     </row>
     <row r="23" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>64</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F23" s="6">
         <v>2</v>
@@ -1745,16 +1742,16 @@
         <v>74</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>85</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F24" s="6">
         <v>2</v>
@@ -1762,19 +1759,19 @@
     </row>
     <row r="25" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>64</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="F25" s="6">
         <v>2</v>
@@ -1785,16 +1782,16 @@
         <v>83</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>64</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="F26" s="6">
         <v>1</v>
@@ -1805,16 +1802,16 @@
         <v>75</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="F27" s="6">
         <v>1</v>
@@ -1825,16 +1822,16 @@
         <v>79</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>64</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="F28" s="6">
         <v>1</v>
@@ -1845,16 +1842,16 @@
         <v>76</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>64</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="F29" s="6">
         <v>1</v>
@@ -1865,16 +1862,16 @@
         <v>78</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>64</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="F30" s="6">
         <v>1</v>
@@ -1885,16 +1882,16 @@
         <v>73</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>85</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="F31" s="6">
         <v>1</v>
@@ -1905,16 +1902,16 @@
         <v>77</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>64</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="F32" s="6">
         <v>1</v>
@@ -1925,16 +1922,16 @@
         <v>72</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>85</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F33" s="6">
         <v>6</v>
@@ -1945,16 +1942,16 @@
         <v>61</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="F34" s="6">
         <v>1</v>
@@ -1965,16 +1962,16 @@
         <v>62</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="F35" s="6">
         <v>1</v>
@@ -1985,36 +1982,36 @@
         <v>63</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="F36" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="21" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" s="21" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>187</v>
+        <v>210</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>188</v>
+        <v>209</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>189</v>
+        <v>211</v>
       </c>
       <c r="F37" s="6">
         <v>8</v>
@@ -2022,19 +2019,19 @@
     </row>
     <row r="38" spans="1:6" s="21" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E38" s="3" t="s">
         <v>185</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>193</v>
       </c>
       <c r="F38" s="6">
         <v>3</v>
@@ -2045,7 +2042,7 @@
         <v>60</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>65</v>
@@ -2054,7 +2051,7 @@
         <v>85</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="F39" s="6">
         <v>2</v>
@@ -2062,19 +2059,19 @@
     </row>
     <row r="40" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="F40" s="6">
         <v>1</v>
@@ -2082,7 +2079,7 @@
     </row>
     <row r="41" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>44</v>
@@ -2102,19 +2099,19 @@
     </row>
     <row r="42" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="E42" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>104</v>
       </c>
       <c r="F42" s="6">
         <v>1</v>
@@ -2162,19 +2159,19 @@
     </row>
     <row r="45" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B45" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D45" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="E45" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>99</v>
       </c>
       <c r="F45" s="6">
         <v>1</v>
@@ -2185,16 +2182,16 @@
         <v>35</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>36</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F46" s="6">
         <v>1</v>
@@ -2225,16 +2222,16 @@
         <v>50</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="F48" s="6">
         <v>1</v>
@@ -2268,21 +2265,21 @@
       <c r="E50" s="7"/>
       <c r="F50" s="7"/>
     </row>
-    <row r="51" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" s="21" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>93</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>94</v>
+        <v>213</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>109</v>
+        <v>215</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>110</v>
+        <v>214</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>95</v>
+        <v>212</v>
       </c>
       <c r="F51" s="6">
         <v>1</v>
@@ -2290,17 +2287,17 @@
     </row>
     <row r="52" spans="1:6" s="21" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="C52" s="4"/>
       <c r="D52" s="4" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="F52" s="6">
         <v>1</v>
@@ -2308,17 +2305,17 @@
     </row>
     <row r="53" spans="1:6" s="21" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="C53" s="4"/>
       <c r="D53" s="4" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="F53" s="6">
         <v>1</v>
@@ -2326,19 +2323,19 @@
     </row>
     <row r="54" spans="1:6" s="21" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="F54" s="6">
         <v>1</v>
@@ -2359,10 +2356,10 @@
     <hyperlink ref="E46" r:id="rId6" xr:uid="{F31726C3-9FF8-43C7-9350-F158FCF5EC6B}"/>
     <hyperlink ref="E49" r:id="rId7" xr:uid="{C163C681-4A90-4128-86E8-18F6B40729D2}"/>
     <hyperlink ref="E18" r:id="rId8" xr:uid="{62A10723-6D8A-428A-8FC9-08456B2B4C8B}"/>
-    <hyperlink ref="E37" r:id="rId9" display="https://octopart.com/c0603c104k8ractu-kemet-145075?r=sp&amp;s=9bS9ASSwSEqMCE9KBEQZ0g" xr:uid="{54E50179-9B71-4984-BDB7-EF3700D8B5E3}"/>
-    <hyperlink ref="E38" r:id="rId10" xr:uid="{23ED7AA4-FF72-4206-9C6A-9ACA87A02BDE}"/>
-    <hyperlink ref="E41" r:id="rId11" xr:uid="{8FCB3B04-50B6-4789-81C7-E5923FF5710D}"/>
-    <hyperlink ref="E48" r:id="rId12" xr:uid="{4381D6DD-B046-4538-AB71-7916DA04B71C}"/>
+    <hyperlink ref="E38" r:id="rId9" xr:uid="{23ED7AA4-FF72-4206-9C6A-9ACA87A02BDE}"/>
+    <hyperlink ref="E41" r:id="rId10" xr:uid="{8FCB3B04-50B6-4789-81C7-E5923FF5710D}"/>
+    <hyperlink ref="E48" r:id="rId11" xr:uid="{4381D6DD-B046-4538-AB71-7916DA04B71C}"/>
+    <hyperlink ref="E51" r:id="rId12" xr:uid="{D92BC9A1-95C6-4AB0-BEDF-800E397FEE1B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId13"/>

</xml_diff>